<commit_message>
Minor changes to exclude a poorly performing genotype. Also added a manually created workbook that combines the currently complete data, and a simple script to make boxplots for all the measurement variables in a data set.
</commit_message>
<xml_diff>
--- a/Exports/ErrorSummary.xlsx
+++ b/Exports/ErrorSummary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">FilePath</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t xml:space="preserve">NIR_Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oil13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PO13</t>
   </si>
   <si>
     <t xml:space="preserve">protein_dry_basis</t>
@@ -177,9 +186,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:T2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:T2"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:W2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:W2"/>
+  <tableColumns count="23">
     <tableColumn id="1" name="FilePath"/>
     <tableColumn id="2" name="Date"/>
     <tableColumn id="3" name="Test"/>
@@ -190,16 +199,19 @@
     <tableColumn id="8" name="Rep"/>
     <tableColumn id="9" name="Plot"/>
     <tableColumn id="10" name="NIR_Number"/>
-    <tableColumn id="11" name="protein_dry_basis"/>
-    <tableColumn id="12" name="oil_dry_basis"/>
-    <tableColumn id="13" name="protein_plus_oil"/>
-    <tableColumn id="14" name="moisture"/>
-    <tableColumn id="15" name="oil_outlier"/>
-    <tableColumn id="16" name="protein_outlier"/>
-    <tableColumn id="17" name="moisture_outlier"/>
-    <tableColumn id="18" name="oil_var"/>
-    <tableColumn id="19" name="protein_var"/>
-    <tableColumn id="20" name="moisture_var"/>
+    <tableColumn id="11" name="Pro13"/>
+    <tableColumn id="12" name="Oil13"/>
+    <tableColumn id="13" name="PO13"/>
+    <tableColumn id="14" name="protein_dry_basis"/>
+    <tableColumn id="15" name="oil_dry_basis"/>
+    <tableColumn id="16" name="protein_plus_oil"/>
+    <tableColumn id="17" name="moisture"/>
+    <tableColumn id="18" name="oil_outlier"/>
+    <tableColumn id="19" name="protein_outlier"/>
+    <tableColumn id="20" name="moisture_outlier"/>
+    <tableColumn id="21" name="oil_var"/>
+    <tableColumn id="22" name="protein_var"/>
+    <tableColumn id="23" name="moisture_var"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -564,67 +576,85 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="O2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="R2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="S2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="T2" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="U2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" t="s">
+        <v>23</v>
+      </c>
+      <c r="W2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -655,18 +685,18 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
@@ -674,13 +704,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
@@ -688,13 +718,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
@@ -702,13 +732,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D5" t="n">
         <v>2</v>
@@ -716,13 +746,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D6" t="n">
         <v>2</v>
@@ -730,13 +760,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D7" t="n">
         <v>2</v>
@@ -744,13 +774,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
       </c>
       <c r="D8" t="n">
         <v>2</v>
@@ -758,13 +788,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" t="n">
         <v>2</v>
@@ -772,13 +802,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
@@ -786,13 +816,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>

</xml_diff>